<commit_message>
rolled back the changes on the endcash position
</commit_message>
<xml_diff>
--- a/financial_models/Opportunities/Monitor/Monitor.xlsx
+++ b/financial_models/Opportunities/Monitor/Monitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry.chen\PycharmProjects\InvestmentManagement\financial_models\Opportunities\Monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A8CB82-F0B2-44D4-8F18-EE0FD4A9F456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4C2018-E67E-43F6-AAAF-8EEA478F4A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1357,7 +1357,7 @@
   <dimension ref="A2:O200"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,45 +1448,45 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="7">
-        <v>1.9299999475479126</v>
+        <v>20.850000381469727</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="7">
-        <f>E5-H5</f>
-        <v>0.15972063557968785</v>
+        <f t="shared" ref="G5:G11" si="0">E5-H5</f>
+        <v>9.7234781125726144</v>
       </c>
       <c r="H5" s="7">
-        <v>1.7702793119682247</v>
+        <v>11.126522268897112</v>
       </c>
       <c r="I5" s="6">
-        <v>0.48311904251807375</v>
+        <v>-1.6763136715094107E-2</v>
       </c>
       <c r="J5" s="7">
-        <v>1.77</v>
+        <v>17.28</v>
       </c>
       <c r="K5" s="7">
-        <v>2.3092203850174395</v>
+        <v>22.398295553313996</v>
       </c>
       <c r="L5" s="7">
-        <v>2.0268895213531741</v>
+        <v>17.277299528915517</v>
       </c>
       <c r="M5" s="7">
-        <v>2.2798113788959483E-2</v>
+        <v>0.17568614818334663</v>
       </c>
       <c r="N5" s="6">
-        <f>M5/E5</f>
-        <v>1.1812494512201802E-2</v>
+        <f t="shared" ref="N5:N11" si="1">M5/E5</f>
+        <v>8.4261940033097706E-3</v>
       </c>
       <c r="O5" s="8">
         <v>45001</v>
@@ -1494,45 +1494,45 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="7">
-        <v>20.600000381469727</v>
+        <v>1.8200000524520874</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="7">
-        <f>E6-H6</f>
-        <v>9.4734781125726144</v>
+        <f t="shared" si="0"/>
+        <v>1.0189850091005896</v>
       </c>
       <c r="H6" s="7">
-        <v>11.126522268897112</v>
+        <v>0.80101504335149776</v>
       </c>
       <c r="I6" s="6">
-        <v>-6.9052825115742955E-3</v>
+        <v>-0.1628401353480384</v>
       </c>
       <c r="J6" s="7">
-        <v>17.28</v>
+        <v>1.2</v>
       </c>
       <c r="K6" s="7">
-        <v>22.398295553313996</v>
+        <v>1.5970421402726409</v>
       </c>
       <c r="L6" s="7">
-        <v>17.277299528915517</v>
+        <v>0.9934935520797944</v>
       </c>
       <c r="M6" s="7">
-        <v>0.17781826159269129</v>
+        <v>5.2856581562630324E-2</v>
       </c>
       <c r="N6" s="6">
-        <f>M6/E6</f>
-        <v>8.6319542864010702E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.9042076944677343E-2</v>
       </c>
       <c r="O6" s="8">
         <v>45001</v>
@@ -1540,45 +1540,45 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>104</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="7">
-        <v>0.61000001430511475</v>
+        <v>3.2400000095367432</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="7">
-        <f>E7-H7</f>
-        <v>1.4489887365273371</v>
+        <f t="shared" si="0"/>
+        <v>1.5547084618716323</v>
       </c>
       <c r="H7" s="7">
-        <v>-0.83898872222222232</v>
+        <v>1.6852915476651109</v>
       </c>
       <c r="I7" s="6">
-        <v>-2.6337239118644606E-2</v>
+        <v>-0.2020017387979246</v>
       </c>
       <c r="J7" s="7">
-        <v>0.4</v>
+        <v>1.95</v>
       </c>
       <c r="K7" s="7">
-        <v>0.81943800764118024</v>
+        <v>2.5933934417545887</v>
       </c>
       <c r="L7" s="7">
-        <v>0.25787827777777772</v>
+        <v>1.9610728132121873</v>
       </c>
       <c r="M7" s="7">
-        <v>0</v>
+        <v>0.10656816545832766</v>
       </c>
       <c r="N7" s="6">
-        <f>M7/E7</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3.2891408995262571E-2</v>
       </c>
       <c r="O7" s="8">
         <v>45001</v>
@@ -1586,45 +1586,45 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="7">
-        <v>3.5499999523162842</v>
+        <v>6.8499999046325684</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="7">
-        <f>E8-H8</f>
-        <v>3.173371256600082</v>
+        <f t="shared" si="0"/>
+        <v>6.2726984761467675</v>
       </c>
       <c r="H8" s="7">
-        <v>0.37662869571620239</v>
+        <v>0.57730142848580079</v>
       </c>
       <c r="I8" s="6">
-        <v>-3.1146088749145096E-2</v>
+        <v>-0.11019497191780214</v>
       </c>
       <c r="J8" s="7">
-        <v>2.9</v>
+        <v>5.2</v>
       </c>
       <c r="K8" s="7">
-        <v>4.4299945978942814</v>
+        <v>6.6096946305743813</v>
       </c>
       <c r="L8" s="7">
-        <v>-1.6019094395779059</v>
+        <v>2.1139700509567434</v>
       </c>
       <c r="M8" s="7">
-        <v>5.8527900015945961E-2</v>
+        <v>2.1001006800062248E-2</v>
       </c>
       <c r="N8" s="6">
-        <f>M8/E8</f>
-        <v>1.6486732620308347E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.0658404514516172E-3</v>
       </c>
       <c r="O8" s="8">
         <v>45001</v>
@@ -1632,45 +1632,45 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="7">
-        <v>6.8299999237060547</v>
+        <v>3.5699999332427979</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="7">
-        <f>E9-H9</f>
-        <v>6.2519959364391475</v>
+        <f t="shared" si="0"/>
+        <v>3.1933712375265957</v>
       </c>
       <c r="H9" s="7">
-        <v>0.57800398726690694</v>
+        <v>0.37662869571620239</v>
       </c>
       <c r="I9" s="6">
-        <v>-0.10804430500150497</v>
+        <v>-3.4124134660860866E-2</v>
       </c>
       <c r="J9" s="7">
-        <v>5.2</v>
+        <v>2.9</v>
       </c>
       <c r="K9" s="7">
-        <v>6.6103971893554885</v>
+        <v>4.4299945978942814</v>
       </c>
       <c r="L9" s="7">
-        <v>2.1146726097378492</v>
+        <v>-1.6019094395779059</v>
       </c>
       <c r="M9" s="7">
-        <v>2.1062503101691915E-2</v>
+        <v>5.8200012927465114E-2</v>
       </c>
       <c r="N9" s="6">
-        <f>M9/E9</f>
-        <v>3.0838218648563472E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.6302524934391056E-2</v>
       </c>
       <c r="O9" s="8">
         <v>45001</v>
@@ -1678,45 +1678,45 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="7">
-        <v>1.8400000333786011</v>
+        <v>0.60000002384185791</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="7">
-        <f>E10-H10</f>
-        <v>1.0391719330785629</v>
+        <f t="shared" si="0"/>
+        <v>1.4389887460640802</v>
       </c>
       <c r="H10" s="7">
-        <v>0.80082810030003815</v>
+        <v>-0.83898872222222232</v>
       </c>
       <c r="I10" s="6">
-        <v>-0.17017664147140771</v>
+        <v>-2.2426662111525358E-2</v>
       </c>
       <c r="J10" s="7">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="K10" s="7">
-        <v>1.5968551972211811</v>
+        <v>0.81943800764118024</v>
       </c>
       <c r="L10" s="7">
-        <v>0.99330660902833467</v>
+        <v>0.25787827777777772</v>
       </c>
       <c r="M10" s="7">
-        <v>5.2282054060501848E-2</v>
+        <v>0</v>
       </c>
       <c r="N10" s="6">
-        <f>M10/E10</f>
-        <v>2.8414159300041826E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O10" s="8">
         <v>45001</v>
@@ -1724,45 +1724,45 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="7">
-        <v>3.2400000095367432</v>
+        <v>1.8999999761581421</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="7">
-        <f>E11-H11</f>
-        <v>1.5547084618716323</v>
+        <f t="shared" si="0"/>
+        <v>0.12972066418991735</v>
       </c>
       <c r="H11" s="7">
-        <v>1.6852915476651109</v>
+        <v>1.7702793119682247</v>
       </c>
       <c r="I11" s="6">
-        <v>-0.2020017387979246</v>
+        <v>0.59498285502339665</v>
       </c>
       <c r="J11" s="7">
-        <v>1.95</v>
+        <v>1.77</v>
       </c>
       <c r="K11" s="7">
-        <v>2.5933934417545887</v>
+        <v>2.3092203850174395</v>
       </c>
       <c r="L11" s="7">
-        <v>1.9610728132121873</v>
+        <v>2.0268895213531741</v>
       </c>
       <c r="M11" s="7">
-        <v>0.10656816545832766</v>
+        <v>2.315808366790257E-2</v>
       </c>
       <c r="N11" s="6">
-        <f>M11/E11</f>
-        <v>3.2891408995262571E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.2188465241314856E-2</v>
       </c>
       <c r="O11" s="8">
         <v>45001</v>
@@ -4803,7 +4803,7 @@
   <dimension ref="A2:J200"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6854,8 +6854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB6B1BF-BEDD-44AB-AFC3-888836F1C221}">
   <dimension ref="A2:F48"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>